<commit_message>
Update annotation guidelines, calculate semantic similarity for collocations
</commit_message>
<xml_diff>
--- a/gold-std/gold-std-anna-todo.xlsx
+++ b/gold-std/gold-std-anna-todo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Liz (Casual)\Documents\UniPotsdam\S1 (WS1920)\BM1_ANLP\nlp-taboo-implementation\gold-std\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F74A088C-30B4-4A63-A5DF-BB9326A722D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC0FD084-C1A6-4334-994C-FC4FBDB971E3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3940,7 +3940,7 @@
   <dimension ref="A1:J1201"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -4060,7 +4060,7 @@
       <c r="B8" t="s">
         <v>18</v>
       </c>
-      <c r="G8">
+      <c r="C8">
         <v>1</v>
       </c>
     </row>
@@ -4071,7 +4071,7 @@
       <c r="B9" t="s">
         <v>19</v>
       </c>
-      <c r="G9">
+      <c r="J9">
         <v>1</v>
       </c>
     </row>

</xml_diff>